<commit_message>
Added column range ("A:B") type parsing
</commit_message>
<xml_diff>
--- a/Office.IO.Tests/Tests.xlsx
+++ b/Office.IO.Tests/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\GitHub\bartelsk\Office.IO\Office.IO.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357A4A45-2611-4877-81D2-DF1B6174D564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E51CBE1-8742-41C1-B407-A964073D7CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="16005" windowHeight="12420" xr2:uid="{CBD9BA64-4CED-4F54-94D9-C2D2B951ACBB}"/>
+    <workbookView xWindow="7995" yWindow="4665" windowWidth="16005" windowHeight="12420" xr2:uid="{CBD9BA64-4CED-4F54-94D9-C2D2B951ACBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,83 +435,85 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEAD468-834D-430B-AFA3-03C4284E4E85}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>23</v>
       </c>
       <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>45</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>58.932000000000002</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="K4" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="L4" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -519,13 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
         <v>14</v>
       </c>

</xml_diff>